<commit_message>
Correction for the delete operation on budget
</commit_message>
<xml_diff>
--- a/Doc/testsApplication/fichier de test.xlsx
+++ b/Doc/testsApplication/fichier de test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80494D9-7938-425B-947E-E95DA7E8471D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356B8ABD-608F-47B6-916B-93291BA52FF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>création</t>
   </si>
@@ -248,11 +248,51 @@
     <t>Si aucun compte par défaut n'existe, le dashboard ne remplit pas le résumé</t>
   </si>
   <si>
-    <t>Catégories</t>
-  </si>
-  <si>
-    <t>Catégories 
-de budget</t>
+    <t>La création d'un budget avec une valeur de plafond négative la convertit 
+en positif</t>
+  </si>
+  <si>
+    <t>Création avec une date de fin inférieure à la date de début</t>
+  </si>
+  <si>
+    <t>Création d'un budget</t>
+  </si>
+  <si>
+    <t>La modification d'un budget avec une valeur de plafond négative la 
+convertit en positif</t>
+  </si>
+  <si>
+    <t>Modification avec une date de fin inférieure à la date de début</t>
+  </si>
+  <si>
+    <t>Modification d'un budget</t>
+  </si>
+  <si>
+    <t>Suppression d'un budget</t>
+  </si>
+  <si>
+    <t>Création d'un budget avec plusieurs catégories</t>
+  </si>
+  <si>
+    <t>Modification des catégories d'un budget</t>
+  </si>
+  <si>
+    <t>Suppression des catégories d'un budget</t>
+  </si>
+  <si>
+    <t>Création d'un budget partagé avec plusieurs participants</t>
+  </si>
+  <si>
+    <t>Modification des participants d'un budget partagé</t>
+  </si>
+  <si>
+    <t>Suppression des participants d'un budget partagé</t>
+  </si>
+  <si>
+    <t>Catégories du budget</t>
+  </si>
+  <si>
+    <t>Participants du budget partagé</t>
   </si>
 </sst>
 </file>
@@ -393,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -523,8 +563,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1556,112 +1606,254 @@
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="48" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="D56" s="56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="56"/>
+      <c r="F56" s="55"/>
+    </row>
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="49"/>
+      <c r="C57" s="16" t="s">
         <v>74</v>
       </c>
+      <c r="D57" s="9">
+        <v>1</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B58" s="49"/>
+      <c r="C58" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D58" s="9">
+        <v>0</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
-      <c r="B59" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="B59" s="50"/>
+      <c r="C59" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="10">
+        <v>1</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="8"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="57">
+        <v>0</v>
+      </c>
+      <c r="E60" s="57"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+      <c r="B61" s="41"/>
+      <c r="C61" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="19">
+        <v>1</v>
+      </c>
+      <c r="E61" s="19"/>
+      <c r="F61" s="58"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+      <c r="B62" s="41"/>
+      <c r="C62" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" s="19">
+        <v>0</v>
+      </c>
+      <c r="E62" s="19"/>
+      <c r="F62" s="58"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="12">
+        <v>1</v>
+      </c>
+      <c r="E63" s="12"/>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="56">
+        <v>1</v>
+      </c>
+      <c r="E64" s="56"/>
+      <c r="F64" s="55"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="9">
+        <v>1</v>
+      </c>
+      <c r="E65" s="9"/>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D66" s="10">
+        <v>1</v>
+      </c>
+      <c r="E66" s="10"/>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" s="11">
+        <v>1</v>
+      </c>
+      <c r="E67" s="11"/>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="54"/>
+      <c r="C68" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="11">
+        <v>1</v>
+      </c>
+      <c r="E68" s="11"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="42"/>
+      <c r="C69" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="12">
+        <v>1</v>
+      </c>
+      <c r="E69" s="12"/>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="59" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="B67" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+      <c r="C70" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="61">
+        <v>1</v>
+      </c>
+      <c r="E70" s="61"/>
+      <c r="F70" s="60"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>8</v>
-      </c>
-      <c r="B73" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>9</v>
-      </c>
-      <c r="B78" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" t="str">
+      <c r="C78" t="str">
         <f>"-&gt; plusieurs cas"</f>
         <v>-&gt; plusieurs cas</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>8</v>
+      </c>
+      <c r="B80" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>5</v>
       </c>
-      <c r="B83" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="21">
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
     <mergeCell ref="B2:B8"/>
     <mergeCell ref="B9:B17"/>
     <mergeCell ref="B18:B20"/>

</xml_diff>

<commit_message>
File of tests finished
</commit_message>
<xml_diff>
--- a/Doc/testsApplication/fichier de test.xlsx
+++ b/Doc/testsApplication/fichier de test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195BC43A-0DCF-48C6-8275-C5B1D1034804}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F19AB6-7F0A-413B-8085-19ADEB4D7F7D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
   <si>
     <t>Client</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t>Modification d'une créance complète</t>
+  </si>
+  <si>
+    <t>Suppression d'une dette</t>
+  </si>
+  <si>
+    <t>Suppression d'une créance</t>
   </si>
 </sst>
 </file>
@@ -507,9 +513,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -669,9 +674,59 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -981,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96:F96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,59 +1047,59 @@
     <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="21" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="85" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="36" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="58" t="s">
+      <c r="A2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="39">
-        <v>0</v>
-      </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="23"/>
+      <c r="D2" s="38">
+        <v>0</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="24" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="25">
-        <v>0</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="H3" s="9">
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="H3" s="8">
         <v>0</v>
       </c>
       <c r="I3" t="s">
@@ -1052,17 +1107,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="24" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="25">
-        <v>0</v>
-      </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="H4" s="9">
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="H4" s="8">
         <v>1</v>
       </c>
       <c r="I4" t="s">
@@ -1070,1147 +1125,1207 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="24" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="28">
-        <v>0</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="D5" s="27">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="51"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="26" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="27">
-        <v>0</v>
-      </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="D6" s="26">
+        <v>0</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="26" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="27">
-        <v>1</v>
-      </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="31" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="32">
-        <v>1</v>
-      </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
+      <c r="D8" s="31">
+        <v>1</v>
+      </c>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="59" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="34">
-        <v>0</v>
-      </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="35" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="36">
-        <v>0</v>
-      </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="D10" s="35">
+        <v>0</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="35" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="36">
-        <v>0</v>
-      </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="35">
+        <v>0</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="35" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="36">
-        <v>0</v>
-      </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="35">
+        <v>0</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="35" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="36">
-        <v>0</v>
-      </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="35">
+        <v>0</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="35" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="36">
-        <v>1</v>
-      </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="35">
+        <v>1</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="35" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="36">
-        <v>1</v>
-      </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+      <c r="D15" s="35">
+        <v>1</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="29" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="30">
-        <v>1</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
+      <c r="D16" s="29">
+        <v>1</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="12">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="11">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
-      <c r="B18" s="53" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="23">
-        <v>0</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
+      <c r="D18" s="22">
+        <v>0</v>
+      </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="24" t="s">
+      <c r="A19" s="50"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="25">
-        <v>1</v>
-      </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="D19" s="24">
+        <v>1</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="8" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="10">
-        <v>1</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
+      <c r="D20" s="9">
+        <v>1</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="50"/>
+      <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="14">
-        <v>1</v>
-      </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="D21" s="13">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="53" t="s">
+      <c r="A22" s="50"/>
+      <c r="B22" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="23">
-        <v>1</v>
-      </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
+      <c r="D22" s="22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="7" t="s">
+      <c r="A23" s="50"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="13">
-        <v>0</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="D23" s="12">
+        <v>0</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="15"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="69"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="53" t="s">
+      <c r="A25" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="23">
-        <v>1</v>
-      </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
+      <c r="D25" s="22">
+        <v>1</v>
+      </c>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="64"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="24" t="s">
+      <c r="A26" s="63"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="25">
-        <v>0</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="D26" s="24">
+        <v>0</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="8" t="s">
+      <c r="A27" s="50"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="10">
-        <v>1</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
-      <c r="B28" s="59" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="34">
-        <v>0</v>
-      </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="D28" s="33">
+        <v>0</v>
+      </c>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="29" t="s">
+      <c r="A29" s="50"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="30">
-        <v>1</v>
-      </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
+      <c r="D29" s="29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="4" t="s">
+      <c r="A30" s="50"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="12">
-        <v>1</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="D30" s="11">
+        <v>1</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="63" t="s">
+      <c r="A31" s="50"/>
+      <c r="B31" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="23">
-        <v>1</v>
-      </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="D31" s="22">
+        <v>1</v>
+      </c>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="24" t="s">
+      <c r="A32" s="50"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="25">
-        <v>0</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
+      <c r="D32" s="24">
+        <v>0</v>
+      </c>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="17" t="s">
+      <c r="A33" s="51"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="13">
-        <v>1</v>
-      </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="D33" s="12">
+        <v>1</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="15"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="69"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="53" t="s">
+      <c r="B35" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="23">
-        <v>0</v>
-      </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="D35" s="22">
+        <v>0</v>
+      </c>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="66"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="24" t="s">
+      <c r="A36" s="65"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="25">
-        <v>1</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="D36" s="24">
+        <v>1</v>
+      </c>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="51"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="19" t="s">
+      <c r="A37" s="50"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="10">
-        <v>1</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
+      <c r="D37" s="9">
+        <v>1</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="51"/>
-      <c r="B38" s="59" t="s">
+      <c r="A38" s="50"/>
+      <c r="B38" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="20">
-        <v>1</v>
-      </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
+      <c r="D38" s="19">
+        <v>1</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="51"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="3" t="s">
+      <c r="A39" s="50"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="20">
-        <v>1</v>
-      </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
+      <c r="D39" s="19">
+        <v>1</v>
+      </c>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="51"/>
-      <c r="B40" s="53" t="s">
+      <c r="A40" s="50"/>
+      <c r="B40" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="22" t="s">
+      <c r="C40" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="23">
-        <v>0</v>
-      </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
+      <c r="D40" s="22">
+        <v>0</v>
+      </c>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="51"/>
-      <c r="B41" s="58"/>
-      <c r="C41" s="24" t="s">
+      <c r="A41" s="50"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="25">
-        <v>1</v>
-      </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
+      <c r="D41" s="24">
+        <v>1</v>
+      </c>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="51"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="19" t="s">
+      <c r="A42" s="50"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="10">
-        <v>1</v>
-      </c>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="D42" s="9">
+        <v>1</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="52"/>
-      <c r="B43" s="41" t="s">
+      <c r="A43" s="51"/>
+      <c r="B43" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="11">
-        <v>1</v>
-      </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
+      <c r="D43" s="10">
+        <v>1</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="15"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="69"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="50" t="s">
+      <c r="A45" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="23">
-        <v>0</v>
-      </c>
-      <c r="E45" s="23"/>
-      <c r="F45" s="22"/>
+      <c r="D45" s="22">
+        <v>0</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="70"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="51"/>
-      <c r="B46" s="58"/>
-      <c r="C46" s="24" t="s">
+      <c r="A46" s="50"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="25">
-        <v>1</v>
-      </c>
-      <c r="E46" s="25"/>
-      <c r="F46" s="24"/>
+      <c r="D46" s="24">
+        <v>1</v>
+      </c>
+      <c r="E46" s="24"/>
+      <c r="F46" s="71"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="51"/>
-      <c r="B47" s="58"/>
-      <c r="C47" s="24" t="s">
+      <c r="A47" s="50"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D47" s="25">
-        <v>1</v>
-      </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="24"/>
+      <c r="D47" s="24">
+        <v>1</v>
+      </c>
+      <c r="E47" s="24"/>
+      <c r="F47" s="71"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="51"/>
-      <c r="B48" s="54"/>
-      <c r="C48" s="8" t="s">
+      <c r="A48" s="50"/>
+      <c r="B48" s="53"/>
+      <c r="C48" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="10">
-        <v>1</v>
-      </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="8"/>
+      <c r="D48" s="9">
+        <v>1</v>
+      </c>
+      <c r="E48" s="9"/>
+      <c r="F48" s="72"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="51"/>
-      <c r="B49" s="60" t="s">
+      <c r="A49" s="50"/>
+      <c r="B49" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="30">
-        <v>0</v>
-      </c>
-      <c r="E49" s="30"/>
-      <c r="F49" s="29"/>
+      <c r="D49" s="29">
+        <v>0</v>
+      </c>
+      <c r="E49" s="29"/>
+      <c r="F49" s="73"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="51"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="35" t="s">
+      <c r="A50" s="50"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D50" s="36">
-        <v>1</v>
-      </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="35"/>
+      <c r="D50" s="35">
+        <v>1</v>
+      </c>
+      <c r="E50" s="35"/>
+      <c r="F50" s="74"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="51"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="35" t="s">
+      <c r="A51" s="50"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="36">
-        <v>1</v>
-      </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="35"/>
+      <c r="D51" s="35">
+        <v>1</v>
+      </c>
+      <c r="E51" s="35"/>
+      <c r="F51" s="74"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="51"/>
-      <c r="B52" s="61"/>
-      <c r="C52" s="4" t="s">
+      <c r="A52" s="50"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="12">
-        <v>1</v>
-      </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="4"/>
+      <c r="D52" s="11">
+        <v>1</v>
+      </c>
+      <c r="E52" s="11"/>
+      <c r="F52" s="75"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="51"/>
-      <c r="B53" s="63" t="s">
+      <c r="A53" s="50"/>
+      <c r="B53" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="27">
-        <v>1</v>
-      </c>
-      <c r="E53" s="27"/>
-      <c r="F53" s="26"/>
+      <c r="D53" s="26">
+        <v>1</v>
+      </c>
+      <c r="E53" s="26"/>
+      <c r="F53" s="76"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="52"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="18" t="s">
+      <c r="A54" s="51"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="13">
-        <v>1</v>
-      </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="18"/>
+      <c r="D54" s="12">
+        <v>1</v>
+      </c>
+      <c r="E54" s="12"/>
+      <c r="F54" s="77"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="15"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="15"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="69"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="50" t="s">
+      <c r="A56" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C56" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="23">
-        <v>0</v>
-      </c>
-      <c r="E56" s="23"/>
-      <c r="F56" s="22"/>
+      <c r="D56" s="22">
+        <v>0</v>
+      </c>
+      <c r="E56" s="22"/>
+      <c r="F56" s="70"/>
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="51"/>
-      <c r="B57" s="58"/>
-      <c r="C57" s="47" t="s">
+      <c r="A57" s="50"/>
+      <c r="B57" s="57"/>
+      <c r="C57" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="D57" s="25">
-        <v>1</v>
-      </c>
-      <c r="E57" s="25"/>
-      <c r="F57" s="24"/>
+      <c r="D57" s="24">
+        <v>1</v>
+      </c>
+      <c r="E57" s="24"/>
+      <c r="F57" s="71"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="51"/>
-      <c r="B58" s="58"/>
-      <c r="C58" s="24" t="s">
+      <c r="A58" s="50"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D58" s="25">
-        <v>0</v>
-      </c>
-      <c r="E58" s="25"/>
-      <c r="F58" s="24"/>
+      <c r="D58" s="24">
+        <v>0</v>
+      </c>
+      <c r="E58" s="24"/>
+      <c r="F58" s="71"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="51"/>
-      <c r="B59" s="54"/>
-      <c r="C59" s="8" t="s">
+      <c r="A59" s="50"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D59" s="10">
-        <v>1</v>
-      </c>
-      <c r="E59" s="10"/>
-      <c r="F59" s="8"/>
+      <c r="D59" s="9">
+        <v>1</v>
+      </c>
+      <c r="E59" s="9"/>
+      <c r="F59" s="72"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="51"/>
-      <c r="B60" s="59" t="s">
+      <c r="A60" s="50"/>
+      <c r="B60" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="33" t="s">
+      <c r="C60" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="D60" s="34">
-        <v>0</v>
-      </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="33"/>
+      <c r="D60" s="33">
+        <v>0</v>
+      </c>
+      <c r="E60" s="33"/>
+      <c r="F60" s="78"/>
     </row>
     <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="51"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="48" t="s">
+      <c r="A61" s="50"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="D61" s="36">
-        <v>1</v>
-      </c>
-      <c r="E61" s="36"/>
-      <c r="F61" s="35"/>
+      <c r="D61" s="35">
+        <v>1</v>
+      </c>
+      <c r="E61" s="35"/>
+      <c r="F61" s="74"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="51"/>
-      <c r="B62" s="60"/>
-      <c r="C62" s="35" t="s">
+      <c r="A62" s="50"/>
+      <c r="B62" s="59"/>
+      <c r="C62" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D62" s="36">
-        <v>0</v>
-      </c>
-      <c r="E62" s="36"/>
-      <c r="F62" s="35"/>
+      <c r="D62" s="35">
+        <v>0</v>
+      </c>
+      <c r="E62" s="35"/>
+      <c r="F62" s="74"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="51"/>
-      <c r="B63" s="61"/>
-      <c r="C63" s="4" t="s">
+      <c r="A63" s="50"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D63" s="12">
-        <v>1</v>
-      </c>
-      <c r="E63" s="12"/>
-      <c r="F63" s="4"/>
+      <c r="D63" s="11">
+        <v>1</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="75"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="51"/>
-      <c r="B64" s="53" t="s">
+      <c r="A64" s="50"/>
+      <c r="B64" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="22" t="s">
+      <c r="C64" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D64" s="23">
-        <v>1</v>
-      </c>
-      <c r="E64" s="23"/>
-      <c r="F64" s="22"/>
+      <c r="D64" s="22">
+        <v>1</v>
+      </c>
+      <c r="E64" s="22"/>
+      <c r="F64" s="70"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="51"/>
-      <c r="B65" s="58"/>
-      <c r="C65" s="24" t="s">
+      <c r="A65" s="50"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D65" s="25">
-        <v>1</v>
-      </c>
-      <c r="E65" s="25"/>
-      <c r="F65" s="24"/>
+      <c r="D65" s="24">
+        <v>1</v>
+      </c>
+      <c r="E65" s="24"/>
+      <c r="F65" s="71"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="51"/>
-      <c r="B66" s="54"/>
-      <c r="C66" s="8" t="s">
+      <c r="A66" s="50"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D66" s="10">
-        <v>1</v>
-      </c>
-      <c r="E66" s="10"/>
-      <c r="F66" s="8"/>
+      <c r="D66" s="9">
+        <v>1</v>
+      </c>
+      <c r="E66" s="9"/>
+      <c r="F66" s="72"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="51"/>
-      <c r="B67" s="59" t="s">
+      <c r="A67" s="50"/>
+      <c r="B67" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C67" s="33" t="s">
+      <c r="C67" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="D67" s="34">
-        <v>1</v>
-      </c>
-      <c r="E67" s="34"/>
-      <c r="F67" s="33"/>
+      <c r="D67" s="33">
+        <v>1</v>
+      </c>
+      <c r="E67" s="33"/>
+      <c r="F67" s="78"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="51"/>
-      <c r="B68" s="62"/>
-      <c r="C68" s="35" t="s">
+      <c r="A68" s="50"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="D68" s="36">
-        <v>1</v>
-      </c>
-      <c r="E68" s="36"/>
-      <c r="F68" s="35"/>
+      <c r="D68" s="35">
+        <v>1</v>
+      </c>
+      <c r="E68" s="35"/>
+      <c r="F68" s="74"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="51"/>
-      <c r="B69" s="60"/>
-      <c r="C69" s="42" t="s">
+      <c r="A69" s="50"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="D69" s="20">
-        <v>1</v>
-      </c>
-      <c r="E69" s="20"/>
-      <c r="F69" s="42"/>
+      <c r="D69" s="19">
+        <v>1</v>
+      </c>
+      <c r="E69" s="19"/>
+      <c r="F69" s="79"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="51"/>
-      <c r="B70" s="53" t="s">
+      <c r="A70" s="50"/>
+      <c r="B70" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C70" s="22" t="s">
+      <c r="C70" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D70" s="23">
-        <v>1</v>
-      </c>
-      <c r="E70" s="23"/>
-      <c r="F70" s="22"/>
+      <c r="D70" s="22">
+        <v>1</v>
+      </c>
+      <c r="E70" s="22"/>
+      <c r="F70" s="70"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="51"/>
-      <c r="B71" s="58"/>
-      <c r="C71" s="24" t="s">
+      <c r="A71" s="50"/>
+      <c r="B71" s="57"/>
+      <c r="C71" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D71" s="25">
-        <v>1</v>
-      </c>
-      <c r="E71" s="25"/>
-      <c r="F71" s="24"/>
+      <c r="D71" s="24">
+        <v>1</v>
+      </c>
+      <c r="E71" s="24"/>
+      <c r="F71" s="71"/>
     </row>
     <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="51"/>
-      <c r="B72" s="58"/>
-      <c r="C72" s="47" t="s">
+      <c r="A72" s="50"/>
+      <c r="B72" s="57"/>
+      <c r="C72" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="D72" s="25">
-        <v>1</v>
-      </c>
-      <c r="E72" s="25"/>
-      <c r="F72" s="24"/>
+      <c r="D72" s="24">
+        <v>1</v>
+      </c>
+      <c r="E72" s="24"/>
+      <c r="F72" s="71"/>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="52"/>
-      <c r="B73" s="54"/>
-      <c r="C73" s="19" t="s">
+      <c r="A73" s="51"/>
+      <c r="B73" s="53"/>
+      <c r="C73" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="10">
-        <v>1</v>
-      </c>
-      <c r="E73" s="10"/>
-      <c r="F73" s="8"/>
+      <c r="D73" s="9">
+        <v>1</v>
+      </c>
+      <c r="E73" s="9"/>
+      <c r="F73" s="72"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="15"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="38"/>
-      <c r="F74" s="15"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="69"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="55" t="s">
+      <c r="A75" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B75" s="53" t="s">
+      <c r="B75" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C75" s="22" t="s">
+      <c r="C75" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D75" s="23">
-        <v>1</v>
-      </c>
-      <c r="E75" s="23">
-        <v>0</v>
-      </c>
-      <c r="F75" s="22" t="s">
+      <c r="D75" s="22">
+        <v>1</v>
+      </c>
+      <c r="E75" s="22">
+        <v>0</v>
+      </c>
+      <c r="F75" s="70" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="56"/>
-      <c r="B76" s="54"/>
-      <c r="C76" s="8" t="s">
+      <c r="A76" s="55"/>
+      <c r="B76" s="53"/>
+      <c r="C76" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D76" s="10">
-        <v>1</v>
-      </c>
-      <c r="E76" s="10">
-        <v>0</v>
-      </c>
-      <c r="F76" s="8" t="s">
+      <c r="D76" s="9">
+        <v>1</v>
+      </c>
+      <c r="E76" s="9">
+        <v>0</v>
+      </c>
+      <c r="F76" s="72" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="56"/>
-      <c r="B77" s="5" t="s">
+      <c r="A77" s="55"/>
+      <c r="B77" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C77" s="43" t="s">
+      <c r="C77" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="D77" s="14">
-        <v>1</v>
-      </c>
-      <c r="E77" s="14">
-        <v>0</v>
-      </c>
-      <c r="F77" s="43" t="s">
+      <c r="D77" s="13">
+        <v>1</v>
+      </c>
+      <c r="E77" s="13">
+        <v>0</v>
+      </c>
+      <c r="F77" s="80" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="56"/>
-      <c r="B78" s="44" t="s">
+      <c r="A78" s="55"/>
+      <c r="B78" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C78" s="45" t="s">
+      <c r="C78" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="D78" s="46">
-        <v>1</v>
-      </c>
-      <c r="E78" s="46">
-        <v>0</v>
-      </c>
-      <c r="F78" s="45" t="s">
+      <c r="D78" s="45">
+        <v>1</v>
+      </c>
+      <c r="E78" s="45">
+        <v>0</v>
+      </c>
+      <c r="F78" s="81" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="57"/>
-      <c r="B79" s="16" t="s">
+      <c r="A79" s="56"/>
+      <c r="B79" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="49" t="s">
+      <c r="C79" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="D79" s="11">
-        <v>1</v>
-      </c>
-      <c r="E79" s="11">
-        <v>0</v>
-      </c>
-      <c r="F79" s="11" t="s">
+      <c r="D79" s="10">
+        <v>1</v>
+      </c>
+      <c r="E79" s="10">
+        <v>0</v>
+      </c>
+      <c r="F79" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="15"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="F80" s="15"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="69"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="53" t="s">
+      <c r="B81" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C81" s="67" t="s">
+      <c r="C81" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="D81" s="68">
-        <v>0</v>
-      </c>
-      <c r="E81" s="68"/>
-      <c r="F81" s="67"/>
+      <c r="D81" s="67">
+        <v>0</v>
+      </c>
+      <c r="E81" s="67"/>
+      <c r="F81" s="82"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="B82" s="58"/>
-      <c r="C82" s="7" t="s">
+      <c r="A82" s="50"/>
+      <c r="B82" s="57"/>
+      <c r="C82" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D82" s="9">
-        <v>0</v>
-      </c>
-      <c r="E82" s="9"/>
-      <c r="F82" s="7"/>
+      <c r="D82" s="8">
+        <v>0</v>
+      </c>
+      <c r="E82" s="8"/>
+      <c r="F82" s="83"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="58"/>
-      <c r="C83" s="7" t="s">
+      <c r="A83" s="50"/>
+      <c r="B83" s="57"/>
+      <c r="C83" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D83" s="9">
-        <v>1</v>
-      </c>
-      <c r="E83" s="9"/>
-      <c r="F83" s="7"/>
+      <c r="D83" s="8">
+        <v>1</v>
+      </c>
+      <c r="E83" s="8"/>
+      <c r="F83" s="83"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="58"/>
-      <c r="C84" s="7" t="s">
+      <c r="A84" s="50"/>
+      <c r="B84" s="57"/>
+      <c r="C84" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D84" s="9">
-        <v>1</v>
-      </c>
-      <c r="E84" s="9"/>
-      <c r="F84" s="7"/>
+      <c r="D84" s="8">
+        <v>1</v>
+      </c>
+      <c r="E84" s="8"/>
+      <c r="F84" s="83"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="58"/>
-      <c r="C85" s="7" t="s">
+      <c r="A85" s="50"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D85" s="9">
-        <v>0</v>
-      </c>
-      <c r="E85" s="9"/>
-      <c r="F85" s="7"/>
+      <c r="D85" s="8">
+        <v>0</v>
+      </c>
+      <c r="E85" s="8"/>
+      <c r="F85" s="83"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="58"/>
-      <c r="C86" s="7" t="s">
+      <c r="A86" s="50"/>
+      <c r="B86" s="57"/>
+      <c r="C86" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D86" s="9">
-        <v>0</v>
-      </c>
-      <c r="E86" s="9"/>
-      <c r="F86" s="7"/>
+      <c r="D86" s="8">
+        <v>0</v>
+      </c>
+      <c r="E86" s="8"/>
+      <c r="F86" s="83"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="58"/>
-      <c r="C87" s="7" t="s">
+      <c r="A87" s="50"/>
+      <c r="B87" s="57"/>
+      <c r="C87" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D87" s="9">
-        <v>1</v>
-      </c>
-      <c r="E87" s="9"/>
-      <c r="F87" s="7"/>
+      <c r="D87" s="8">
+        <v>1</v>
+      </c>
+      <c r="E87" s="8"/>
+      <c r="F87" s="83"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="54"/>
-      <c r="C88" s="8" t="s">
+      <c r="A88" s="50"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D88" s="10">
-        <v>1</v>
-      </c>
-      <c r="E88" s="10"/>
-      <c r="F88" s="8"/>
+      <c r="D88" s="9">
+        <v>1</v>
+      </c>
+      <c r="E88" s="9"/>
+      <c r="F88" s="72"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B89" s="1" t="s">
+      <c r="A89" s="50"/>
+      <c r="B89" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="C89" s="67" t="s">
+      <c r="C89" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D89" s="68">
         <v>0</v>
       </c>
+      <c r="E89" s="10"/>
+      <c r="F89" s="84"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C90" s="7" t="s">
+      <c r="A90" s="50"/>
+      <c r="B90" s="61"/>
+      <c r="C90" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="D90" s="9">
-        <v>0</v>
-      </c>
+      <c r="D90" s="19">
+        <v>0</v>
+      </c>
+      <c r="E90" s="10"/>
+      <c r="F90" s="84"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C91" s="7" t="s">
+      <c r="A91" s="50"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="D91" s="9">
-        <v>1</v>
-      </c>
+      <c r="D91" s="19">
+        <v>1</v>
+      </c>
+      <c r="E91" s="10"/>
+      <c r="F91" s="84"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C92" s="7" t="s">
+      <c r="A92" s="50"/>
+      <c r="B92" s="61"/>
+      <c r="C92" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="D92" s="9">
-        <v>1</v>
-      </c>
+      <c r="D92" s="19">
+        <v>1</v>
+      </c>
+      <c r="E92" s="10"/>
+      <c r="F92" s="84"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C93" s="7" t="s">
+      <c r="A93" s="50"/>
+      <c r="B93" s="61"/>
+      <c r="C93" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="D93" s="9">
-        <v>0</v>
-      </c>
+      <c r="D93" s="19">
+        <v>0</v>
+      </c>
+      <c r="E93" s="10"/>
+      <c r="F93" s="84"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C94" s="7" t="s">
+      <c r="A94" s="50"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="D94" s="9">
-        <v>0</v>
-      </c>
+      <c r="D94" s="19">
+        <v>0</v>
+      </c>
+      <c r="E94" s="10"/>
+      <c r="F94" s="84"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C95" s="7" t="s">
+      <c r="A95" s="50"/>
+      <c r="B95" s="61"/>
+      <c r="C95" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="D95" s="9">
-        <v>1</v>
-      </c>
+      <c r="D95" s="19">
+        <v>1</v>
+      </c>
+      <c r="E95" s="10"/>
+      <c r="F95" s="84"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B96" s="69"/>
-      <c r="C96" s="8" t="s">
+      <c r="A96" s="50"/>
+      <c r="B96" s="60"/>
+      <c r="C96" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D96" s="10">
-        <v>1</v>
-      </c>
-      <c r="E96" s="70"/>
-      <c r="F96" s="69"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B101" s="1" t="s">
+      <c r="D96" s="11">
+        <v>1</v>
+      </c>
+      <c r="E96" s="11"/>
+      <c r="F96" s="75"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="50"/>
+      <c r="B97" s="52" t="s">
         <v>19</v>
       </c>
+      <c r="C97" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D97" s="12">
+        <v>1</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="F97" s="77"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="51"/>
+      <c r="B98" s="53"/>
+      <c r="C98" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="12">
+        <v>1</v>
+      </c>
+      <c r="E98" s="12"/>
+      <c r="F98" s="77"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="29">
     <mergeCell ref="B81:B88"/>
+    <mergeCell ref="B89:B96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A81:A98"/>
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="A45:A54"/>
@@ -2237,7 +2352,16 @@
     <mergeCell ref="B67:B69"/>
     <mergeCell ref="B70:B73"/>
   </mergeCells>
-  <conditionalFormatting sqref="D56:E73 D1:E54 D75:E79 D81:E1048576">
+  <conditionalFormatting sqref="D56:E73 D1:E54 D75:E79 D81:E98 D100:E1048576">
+    <cfRule type="iconSet" priority="11">
+      <iconSet showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="percent" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H4">
     <cfRule type="iconSet" priority="10">
       <iconSet showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2246,8 +2370,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H4">
-    <cfRule type="iconSet" priority="9">
+  <conditionalFormatting sqref="D55:E55">
+    <cfRule type="iconSet" priority="4">
       <iconSet showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="1"/>
@@ -2255,7 +2379,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55:E55">
+  <conditionalFormatting sqref="D74:E74">
     <cfRule type="iconSet" priority="3">
       <iconSet showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2264,7 +2388,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D74:E74">
+  <conditionalFormatting sqref="D80:E80">
     <cfRule type="iconSet" priority="2">
       <iconSet showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2273,7 +2397,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D80:E80">
+  <conditionalFormatting sqref="D99:E99">
     <cfRule type="iconSet" priority="1">
       <iconSet showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>

<commit_message>
Tests updated for Derby
</commit_message>
<xml_diff>
--- a/Doc/testsApplication/fichier de test.xlsx
+++ b/Doc/testsApplication/fichier de test.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F19AB6-7F0A-413B-8085-19ADEB4D7F7D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0F5F24-68C3-42D3-9776-172F634DBB52}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PostgreSQL" sheetId="1" r:id="rId1"/>
+    <sheet name="Derby" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="112">
   <si>
     <t>Client</t>
   </si>
@@ -513,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,56 +620,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -727,6 +683,57 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1038,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1049,7 +1056,7 @@
     <col min="3" max="3" width="63.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" style="20" customWidth="1"/>
     <col min="5" max="5" width="15.21875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="85" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="70" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1073,10 +1080,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="57" t="s">
+      <c r="A2" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="72" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="21" t="s">
@@ -1089,8 +1096,8 @@
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="57"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="23" t="s">
         <v>11</v>
       </c>
@@ -1107,8 +1114,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="57"/>
+      <c r="A4" s="78"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="23" t="s">
         <v>12</v>
       </c>
@@ -1125,8 +1132,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
-      <c r="B5" s="57"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="23" t="s">
         <v>13</v>
       </c>
@@ -1137,8 +1144,8 @@
       <c r="F5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="57"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="25" t="s">
         <v>14</v>
       </c>
@@ -1149,8 +1156,8 @@
       <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="57"/>
+      <c r="A7" s="78"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="25" t="s">
         <v>15</v>
       </c>
@@ -1161,8 +1168,8 @@
       <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="53"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="30" t="s">
         <v>27</v>
       </c>
@@ -1173,8 +1180,8 @@
       <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
-      <c r="B9" s="58" t="s">
+      <c r="A9" s="78"/>
+      <c r="B9" s="74" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="32" t="s">
@@ -1187,8 +1194,8 @@
       <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="61"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="34" t="s">
         <v>16</v>
       </c>
@@ -1199,8 +1206,8 @@
       <c r="F10" s="35"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="61"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="34" t="s">
         <v>22</v>
       </c>
@@ -1211,8 +1218,8 @@
       <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="78"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="34" t="s">
         <v>23</v>
       </c>
@@ -1223,8 +1230,8 @@
       <c r="F12" s="35"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="78"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="34" t="s">
         <v>24</v>
       </c>
@@ -1235,8 +1242,8 @@
       <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="75"/>
       <c r="C14" s="34" t="s">
         <v>26</v>
       </c>
@@ -1247,8 +1254,8 @@
       <c r="F14" s="35"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="61"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="34" t="s">
         <v>25</v>
       </c>
@@ -1259,8 +1266,8 @@
       <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="28" t="s">
         <v>29</v>
       </c>
@@ -1271,8 +1278,8 @@
       <c r="F16" s="29"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="60"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1283,8 +1290,8 @@
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="52" t="s">
+      <c r="A18" s="78"/>
+      <c r="B18" s="71" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="21" t="s">
@@ -1297,8 +1304,8 @@
       <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
-      <c r="B19" s="62"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="81"/>
       <c r="C19" s="23" t="s">
         <v>34</v>
       </c>
@@ -1309,8 +1316,8 @@
       <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="50"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="7" t="s">
         <v>33</v>
       </c>
@@ -1321,7 +1328,7 @@
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
+      <c r="A21" s="78"/>
       <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
@@ -1335,8 +1342,8 @@
       <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="50"/>
-      <c r="B22" s="52" t="s">
+      <c r="A22" s="78"/>
+      <c r="B22" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -1349,8 +1356,8 @@
       <c r="F22" s="22"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
-      <c r="B23" s="62"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="6" t="s">
         <v>37</v>
       </c>
@@ -1366,13 +1373,13 @@
       <c r="C24" s="14"/>
       <c r="D24" s="37"/>
       <c r="E24" s="37"/>
-      <c r="F24" s="69"/>
+      <c r="F24" s="54"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="52" t="s">
+      <c r="A25" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="71" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -1385,8 +1392,8 @@
       <c r="F25" s="22"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="63"/>
-      <c r="B26" s="57"/>
+      <c r="A26" s="84"/>
+      <c r="B26" s="72"/>
       <c r="C26" s="23" t="s">
         <v>56</v>
       </c>
@@ -1397,8 +1404,8 @@
       <c r="F26" s="24"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="50"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="78"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="7" t="s">
         <v>40</v>
       </c>
@@ -1409,8 +1416,8 @@
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="50"/>
-      <c r="B28" s="58" t="s">
+      <c r="A28" s="78"/>
+      <c r="B28" s="74" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="32" t="s">
@@ -1423,8 +1430,8 @@
       <c r="F28" s="33"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="50"/>
-      <c r="B29" s="59"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="28" t="s">
         <v>42</v>
       </c>
@@ -1435,8 +1442,8 @@
       <c r="F29" s="29"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="50"/>
-      <c r="B30" s="60"/>
+      <c r="A30" s="78"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="3" t="s">
         <v>43</v>
       </c>
@@ -1447,8 +1454,8 @@
       <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="50"/>
-      <c r="B31" s="62" t="s">
+      <c r="A31" s="78"/>
+      <c r="B31" s="81" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="21" t="s">
@@ -1461,8 +1468,8 @@
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="50"/>
-      <c r="B32" s="62"/>
+      <c r="A32" s="78"/>
+      <c r="B32" s="81"/>
       <c r="C32" s="23" t="s">
         <v>45</v>
       </c>
@@ -1473,8 +1480,8 @@
       <c r="F32" s="24"/>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="51"/>
-      <c r="B33" s="62"/>
+      <c r="A33" s="79"/>
+      <c r="B33" s="81"/>
       <c r="C33" s="16" t="s">
         <v>48</v>
       </c>
@@ -1490,13 +1497,13 @@
       <c r="C34" s="14"/>
       <c r="D34" s="37"/>
       <c r="E34" s="37"/>
-      <c r="F34" s="69"/>
+      <c r="F34" s="54"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="64" t="s">
+      <c r="A35" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="71" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="21" t="s">
@@ -1509,8 +1516,8 @@
       <c r="F35" s="22"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="65"/>
-      <c r="B36" s="57"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="23" t="s">
         <v>49</v>
       </c>
@@ -1521,8 +1528,8 @@
       <c r="F36" s="24"/>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="50"/>
-      <c r="B37" s="53"/>
+      <c r="A37" s="78"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="18" t="s">
         <v>50</v>
       </c>
@@ -1533,8 +1540,8 @@
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="50"/>
-      <c r="B38" s="58" t="s">
+      <c r="A38" s="78"/>
+      <c r="B38" s="74" t="s">
         <v>54</v>
       </c>
       <c r="C38" s="39" t="s">
@@ -1547,8 +1554,8 @@
       <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="50"/>
-      <c r="B39" s="60"/>
+      <c r="A39" s="78"/>
+      <c r="B39" s="76"/>
       <c r="C39" s="2" t="s">
         <v>67</v>
       </c>
@@ -1559,8 +1566,8 @@
       <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="50"/>
-      <c r="B40" s="52" t="s">
+      <c r="A40" s="78"/>
+      <c r="B40" s="71" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="21" t="s">
@@ -1573,8 +1580,8 @@
       <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="50"/>
-      <c r="B41" s="57"/>
+      <c r="A41" s="78"/>
+      <c r="B41" s="72"/>
       <c r="C41" s="23" t="s">
         <v>51</v>
       </c>
@@ -1585,8 +1592,8 @@
       <c r="F41" s="24"/>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="50"/>
-      <c r="B42" s="53"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="18" t="s">
         <v>52</v>
       </c>
@@ -1597,7 +1604,7 @@
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="51"/>
+      <c r="A43" s="79"/>
       <c r="B43" s="40" t="s">
         <v>19</v>
       </c>
@@ -1616,13 +1623,13 @@
       <c r="C44" s="14"/>
       <c r="D44" s="37"/>
       <c r="E44" s="37"/>
-      <c r="F44" s="69"/>
+      <c r="F44" s="54"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="71" t="s">
         <v>38</v>
       </c>
       <c r="C45" s="21" t="s">
@@ -1632,11 +1639,11 @@
         <v>0</v>
       </c>
       <c r="E45" s="22"/>
-      <c r="F45" s="70"/>
+      <c r="F45" s="55"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="50"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="78"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="23" t="s">
         <v>58</v>
       </c>
@@ -1644,11 +1651,11 @@
         <v>1</v>
       </c>
       <c r="E46" s="24"/>
-      <c r="F46" s="71"/>
+      <c r="F46" s="56"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="50"/>
-      <c r="B47" s="57"/>
+      <c r="A47" s="78"/>
+      <c r="B47" s="72"/>
       <c r="C47" s="23" t="s">
         <v>59</v>
       </c>
@@ -1656,11 +1663,11 @@
         <v>1</v>
       </c>
       <c r="E47" s="24"/>
-      <c r="F47" s="71"/>
+      <c r="F47" s="56"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
-      <c r="B48" s="53"/>
+      <c r="A48" s="78"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="7" t="s">
         <v>60</v>
       </c>
@@ -1668,11 +1675,11 @@
         <v>1</v>
       </c>
       <c r="E48" s="9"/>
-      <c r="F48" s="72"/>
+      <c r="F48" s="57"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="50"/>
-      <c r="B49" s="59" t="s">
+      <c r="A49" s="78"/>
+      <c r="B49" s="80" t="s">
         <v>39</v>
       </c>
       <c r="C49" s="28" t="s">
@@ -1682,11 +1689,11 @@
         <v>0</v>
       </c>
       <c r="E49" s="29"/>
-      <c r="F49" s="73"/>
+      <c r="F49" s="58"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="50"/>
-      <c r="B50" s="59"/>
+      <c r="A50" s="78"/>
+      <c r="B50" s="80"/>
       <c r="C50" s="34" t="s">
         <v>61</v>
       </c>
@@ -1694,11 +1701,11 @@
         <v>1</v>
       </c>
       <c r="E50" s="35"/>
-      <c r="F50" s="74"/>
+      <c r="F50" s="59"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="50"/>
-      <c r="B51" s="59"/>
+      <c r="A51" s="78"/>
+      <c r="B51" s="80"/>
       <c r="C51" s="34" t="s">
         <v>62</v>
       </c>
@@ -1706,11 +1713,11 @@
         <v>1</v>
       </c>
       <c r="E51" s="35"/>
-      <c r="F51" s="74"/>
+      <c r="F51" s="59"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="50"/>
-      <c r="B52" s="60"/>
+      <c r="A52" s="78"/>
+      <c r="B52" s="76"/>
       <c r="C52" s="3" t="s">
         <v>63</v>
       </c>
@@ -1718,11 +1725,11 @@
         <v>1</v>
       </c>
       <c r="E52" s="11"/>
-      <c r="F52" s="75"/>
+      <c r="F52" s="60"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="50"/>
-      <c r="B53" s="62" t="s">
+      <c r="A53" s="78"/>
+      <c r="B53" s="81" t="s">
         <v>19</v>
       </c>
       <c r="C53" s="25" t="s">
@@ -1732,11 +1739,11 @@
         <v>1</v>
       </c>
       <c r="E53" s="26"/>
-      <c r="F53" s="76"/>
+      <c r="F53" s="61"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="51"/>
-      <c r="B54" s="62"/>
+      <c r="A54" s="79"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="17" t="s">
         <v>65</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="12"/>
-      <c r="F54" s="77"/>
+      <c r="F54" s="62"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="14"/>
@@ -1752,13 +1759,13 @@
       <c r="C55" s="14"/>
       <c r="D55" s="37"/>
       <c r="E55" s="37"/>
-      <c r="F55" s="69"/>
+      <c r="F55" s="54"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="49" t="s">
+      <c r="A56" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="52" t="s">
+      <c r="B56" s="71" t="s">
         <v>38</v>
       </c>
       <c r="C56" s="21" t="s">
@@ -1768,11 +1775,11 @@
         <v>0</v>
       </c>
       <c r="E56" s="22"/>
-      <c r="F56" s="70"/>
+      <c r="F56" s="55"/>
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="50"/>
-      <c r="B57" s="57"/>
+      <c r="A57" s="78"/>
+      <c r="B57" s="72"/>
       <c r="C57" s="46" t="s">
         <v>68</v>
       </c>
@@ -1780,11 +1787,11 @@
         <v>1</v>
       </c>
       <c r="E57" s="24"/>
-      <c r="F57" s="71"/>
+      <c r="F57" s="56"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="50"/>
-      <c r="B58" s="57"/>
+      <c r="A58" s="78"/>
+      <c r="B58" s="72"/>
       <c r="C58" s="23" t="s">
         <v>69</v>
       </c>
@@ -1792,11 +1799,11 @@
         <v>0</v>
       </c>
       <c r="E58" s="24"/>
-      <c r="F58" s="71"/>
+      <c r="F58" s="56"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="50"/>
-      <c r="B59" s="53"/>
+      <c r="A59" s="78"/>
+      <c r="B59" s="73"/>
       <c r="C59" s="7" t="s">
         <v>70</v>
       </c>
@@ -1804,11 +1811,11 @@
         <v>1</v>
       </c>
       <c r="E59" s="9"/>
-      <c r="F59" s="72"/>
+      <c r="F59" s="57"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="50"/>
-      <c r="B60" s="58" t="s">
+      <c r="A60" s="78"/>
+      <c r="B60" s="74" t="s">
         <v>39</v>
       </c>
       <c r="C60" s="32" t="s">
@@ -1818,11 +1825,11 @@
         <v>0</v>
       </c>
       <c r="E60" s="33"/>
-      <c r="F60" s="78"/>
+      <c r="F60" s="63"/>
     </row>
     <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="50"/>
-      <c r="B61" s="59"/>
+      <c r="A61" s="78"/>
+      <c r="B61" s="80"/>
       <c r="C61" s="47" t="s">
         <v>71</v>
       </c>
@@ -1830,11 +1837,11 @@
         <v>1</v>
       </c>
       <c r="E61" s="35"/>
-      <c r="F61" s="74"/>
+      <c r="F61" s="59"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="50"/>
-      <c r="B62" s="59"/>
+      <c r="A62" s="78"/>
+      <c r="B62" s="80"/>
       <c r="C62" s="34" t="s">
         <v>72</v>
       </c>
@@ -1842,11 +1849,11 @@
         <v>0</v>
       </c>
       <c r="E62" s="35"/>
-      <c r="F62" s="74"/>
+      <c r="F62" s="59"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="50"/>
-      <c r="B63" s="60"/>
+      <c r="A63" s="78"/>
+      <c r="B63" s="76"/>
       <c r="C63" s="3" t="s">
         <v>73</v>
       </c>
@@ -1854,11 +1861,11 @@
         <v>1</v>
       </c>
       <c r="E63" s="11"/>
-      <c r="F63" s="75"/>
+      <c r="F63" s="60"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="50"/>
-      <c r="B64" s="52" t="s">
+      <c r="A64" s="78"/>
+      <c r="B64" s="71" t="s">
         <v>80</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -1868,11 +1875,11 @@
         <v>1</v>
       </c>
       <c r="E64" s="22"/>
-      <c r="F64" s="70"/>
+      <c r="F64" s="55"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="50"/>
-      <c r="B65" s="57"/>
+      <c r="A65" s="78"/>
+      <c r="B65" s="72"/>
       <c r="C65" s="23" t="s">
         <v>75</v>
       </c>
@@ -1880,11 +1887,11 @@
         <v>1</v>
       </c>
       <c r="E65" s="24"/>
-      <c r="F65" s="71"/>
+      <c r="F65" s="56"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="50"/>
-      <c r="B66" s="53"/>
+      <c r="A66" s="78"/>
+      <c r="B66" s="73"/>
       <c r="C66" s="7" t="s">
         <v>76</v>
       </c>
@@ -1892,11 +1899,11 @@
         <v>1</v>
       </c>
       <c r="E66" s="9"/>
-      <c r="F66" s="72"/>
+      <c r="F66" s="57"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="50"/>
-      <c r="B67" s="58" t="s">
+      <c r="A67" s="78"/>
+      <c r="B67" s="74" t="s">
         <v>81</v>
       </c>
       <c r="C67" s="32" t="s">
@@ -1906,11 +1913,11 @@
         <v>1</v>
       </c>
       <c r="E67" s="33"/>
-      <c r="F67" s="78"/>
+      <c r="F67" s="63"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="50"/>
-      <c r="B68" s="61"/>
+      <c r="A68" s="78"/>
+      <c r="B68" s="75"/>
       <c r="C68" s="34" t="s">
         <v>78</v>
       </c>
@@ -1918,11 +1925,11 @@
         <v>1</v>
       </c>
       <c r="E68" s="35"/>
-      <c r="F68" s="74"/>
+      <c r="F68" s="59"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="50"/>
-      <c r="B69" s="59"/>
+      <c r="A69" s="78"/>
+      <c r="B69" s="80"/>
       <c r="C69" s="41" t="s">
         <v>79</v>
       </c>
@@ -1930,11 +1937,11 @@
         <v>1</v>
       </c>
       <c r="E69" s="19"/>
-      <c r="F69" s="79"/>
+      <c r="F69" s="64"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="50"/>
-      <c r="B70" s="52" t="s">
+      <c r="A70" s="78"/>
+      <c r="B70" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C70" s="21" t="s">
@@ -1944,11 +1951,11 @@
         <v>1</v>
       </c>
       <c r="E70" s="22"/>
-      <c r="F70" s="70"/>
+      <c r="F70" s="55"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="50"/>
-      <c r="B71" s="57"/>
+      <c r="A71" s="78"/>
+      <c r="B71" s="72"/>
       <c r="C71" s="23" t="s">
         <v>83</v>
       </c>
@@ -1956,11 +1963,11 @@
         <v>1</v>
       </c>
       <c r="E71" s="24"/>
-      <c r="F71" s="71"/>
+      <c r="F71" s="56"/>
     </row>
     <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="50"/>
-      <c r="B72" s="57"/>
+      <c r="A72" s="78"/>
+      <c r="B72" s="72"/>
       <c r="C72" s="46" t="s">
         <v>84</v>
       </c>
@@ -1968,11 +1975,11 @@
         <v>1</v>
       </c>
       <c r="E72" s="24"/>
-      <c r="F72" s="71"/>
+      <c r="F72" s="56"/>
     </row>
     <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="51"/>
-      <c r="B73" s="53"/>
+      <c r="A73" s="79"/>
+      <c r="B73" s="73"/>
       <c r="C73" s="18" t="s">
         <v>85</v>
       </c>
@@ -1980,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="E73" s="9"/>
-      <c r="F73" s="72"/>
+      <c r="F73" s="57"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="14"/>
@@ -1988,13 +1995,13 @@
       <c r="C74" s="14"/>
       <c r="D74" s="37"/>
       <c r="E74" s="37"/>
-      <c r="F74" s="69"/>
+      <c r="F74" s="54"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="54" t="s">
+      <c r="A75" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="B75" s="52" t="s">
+      <c r="B75" s="71" t="s">
         <v>38</v>
       </c>
       <c r="C75" s="21" t="s">
@@ -2006,13 +2013,13 @@
       <c r="E75" s="22">
         <v>0</v>
       </c>
-      <c r="F75" s="70" t="s">
+      <c r="F75" s="55" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="55"/>
-      <c r="B76" s="53"/>
+      <c r="A76" s="86"/>
+      <c r="B76" s="73"/>
       <c r="C76" s="7" t="s">
         <v>88</v>
       </c>
@@ -2022,12 +2029,12 @@
       <c r="E76" s="9">
         <v>0</v>
       </c>
-      <c r="F76" s="72" t="s">
+      <c r="F76" s="57" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="55"/>
+      <c r="A77" s="86"/>
       <c r="B77" s="4" t="s">
         <v>39</v>
       </c>
@@ -2040,12 +2047,12 @@
       <c r="E77" s="13">
         <v>0</v>
       </c>
-      <c r="F77" s="80" t="s">
+      <c r="F77" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="55"/>
+      <c r="A78" s="86"/>
       <c r="B78" s="43" t="s">
         <v>19</v>
       </c>
@@ -2058,12 +2065,12 @@
       <c r="E78" s="45">
         <v>0</v>
       </c>
-      <c r="F78" s="81" t="s">
+      <c r="F78" s="66" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="56"/>
+      <c r="A79" s="87"/>
       <c r="B79" s="15" t="s">
         <v>90</v>
       </c>
@@ -2086,27 +2093,27 @@
       <c r="C80" s="14"/>
       <c r="D80" s="37"/>
       <c r="E80" s="37"/>
-      <c r="F80" s="69"/>
+      <c r="F80" s="54"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="49" t="s">
+      <c r="A81" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B81" s="52" t="s">
+      <c r="B81" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C81" s="66" t="s">
+      <c r="C81" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="D81" s="67">
-        <v>0</v>
-      </c>
-      <c r="E81" s="67"/>
-      <c r="F81" s="82"/>
+      <c r="D81" s="52">
+        <v>0</v>
+      </c>
+      <c r="E81" s="52"/>
+      <c r="F81" s="67"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="50"/>
-      <c r="B82" s="57"/>
+      <c r="A82" s="78"/>
+      <c r="B82" s="72"/>
       <c r="C82" s="6" t="s">
         <v>95</v>
       </c>
@@ -2114,11 +2121,11 @@
         <v>0</v>
       </c>
       <c r="E82" s="8"/>
-      <c r="F82" s="83"/>
+      <c r="F82" s="68"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="50"/>
-      <c r="B83" s="57"/>
+      <c r="A83" s="78"/>
+      <c r="B83" s="72"/>
       <c r="C83" s="6" t="s">
         <v>96</v>
       </c>
@@ -2126,11 +2133,11 @@
         <v>1</v>
       </c>
       <c r="E83" s="8"/>
-      <c r="F83" s="83"/>
+      <c r="F83" s="68"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="50"/>
-      <c r="B84" s="57"/>
+      <c r="A84" s="78"/>
+      <c r="B84" s="72"/>
       <c r="C84" s="6" t="s">
         <v>97</v>
       </c>
@@ -2138,11 +2145,11 @@
         <v>1</v>
       </c>
       <c r="E84" s="8"/>
-      <c r="F84" s="83"/>
+      <c r="F84" s="68"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="50"/>
-      <c r="B85" s="57"/>
+      <c r="A85" s="78"/>
+      <c r="B85" s="72"/>
       <c r="C85" s="6" t="s">
         <v>99</v>
       </c>
@@ -2150,11 +2157,11 @@
         <v>0</v>
       </c>
       <c r="E85" s="8"/>
-      <c r="F85" s="83"/>
+      <c r="F85" s="68"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="50"/>
-      <c r="B86" s="57"/>
+      <c r="A86" s="78"/>
+      <c r="B86" s="72"/>
       <c r="C86" s="6" t="s">
         <v>100</v>
       </c>
@@ -2162,11 +2169,11 @@
         <v>0</v>
       </c>
       <c r="E86" s="8"/>
-      <c r="F86" s="83"/>
+      <c r="F86" s="68"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="50"/>
-      <c r="B87" s="57"/>
+      <c r="A87" s="78"/>
+      <c r="B87" s="72"/>
       <c r="C87" s="6" t="s">
         <v>101</v>
       </c>
@@ -2174,11 +2181,11 @@
         <v>1</v>
       </c>
       <c r="E87" s="8"/>
-      <c r="F87" s="83"/>
+      <c r="F87" s="68"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="50"/>
-      <c r="B88" s="53"/>
+      <c r="A88" s="78"/>
+      <c r="B88" s="73"/>
       <c r="C88" s="7" t="s">
         <v>98</v>
       </c>
@@ -2186,25 +2193,25 @@
         <v>1</v>
       </c>
       <c r="E88" s="9"/>
-      <c r="F88" s="72"/>
+      <c r="F88" s="57"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="50"/>
-      <c r="B89" s="58" t="s">
+      <c r="A89" s="78"/>
+      <c r="B89" s="74" t="s">
         <v>39</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D89" s="68">
+      <c r="D89" s="53">
         <v>0</v>
       </c>
       <c r="E89" s="10"/>
-      <c r="F89" s="84"/>
+      <c r="F89" s="69"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="50"/>
-      <c r="B90" s="61"/>
+      <c r="A90" s="78"/>
+      <c r="B90" s="75"/>
       <c r="C90" s="41" t="s">
         <v>103</v>
       </c>
@@ -2212,11 +2219,11 @@
         <v>0</v>
       </c>
       <c r="E90" s="10"/>
-      <c r="F90" s="84"/>
+      <c r="F90" s="69"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="50"/>
-      <c r="B91" s="61"/>
+      <c r="A91" s="78"/>
+      <c r="B91" s="75"/>
       <c r="C91" s="41" t="s">
         <v>104</v>
       </c>
@@ -2224,11 +2231,11 @@
         <v>1</v>
       </c>
       <c r="E91" s="10"/>
-      <c r="F91" s="84"/>
+      <c r="F91" s="69"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="50"/>
-      <c r="B92" s="61"/>
+      <c r="A92" s="78"/>
+      <c r="B92" s="75"/>
       <c r="C92" s="41" t="s">
         <v>105</v>
       </c>
@@ -2236,11 +2243,11 @@
         <v>1</v>
       </c>
       <c r="E92" s="10"/>
-      <c r="F92" s="84"/>
+      <c r="F92" s="69"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="50"/>
-      <c r="B93" s="61"/>
+      <c r="A93" s="78"/>
+      <c r="B93" s="75"/>
       <c r="C93" s="41" t="s">
         <v>106</v>
       </c>
@@ -2248,11 +2255,11 @@
         <v>0</v>
       </c>
       <c r="E93" s="10"/>
-      <c r="F93" s="84"/>
+      <c r="F93" s="69"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="50"/>
-      <c r="B94" s="61"/>
+      <c r="A94" s="78"/>
+      <c r="B94" s="75"/>
       <c r="C94" s="41" t="s">
         <v>107</v>
       </c>
@@ -2260,11 +2267,11 @@
         <v>0</v>
       </c>
       <c r="E94" s="10"/>
-      <c r="F94" s="84"/>
+      <c r="F94" s="69"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="50"/>
-      <c r="B95" s="61"/>
+      <c r="A95" s="78"/>
+      <c r="B95" s="75"/>
       <c r="C95" s="41" t="s">
         <v>108</v>
       </c>
@@ -2272,11 +2279,11 @@
         <v>1</v>
       </c>
       <c r="E95" s="10"/>
-      <c r="F95" s="84"/>
+      <c r="F95" s="69"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="50"/>
-      <c r="B96" s="60"/>
+      <c r="A96" s="78"/>
+      <c r="B96" s="76"/>
       <c r="C96" s="3" t="s">
         <v>109</v>
       </c>
@@ -2284,11 +2291,11 @@
         <v>1</v>
       </c>
       <c r="E96" s="11"/>
-      <c r="F96" s="75"/>
+      <c r="F96" s="60"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="50"/>
-      <c r="B97" s="52" t="s">
+      <c r="A97" s="78"/>
+      <c r="B97" s="71" t="s">
         <v>19</v>
       </c>
       <c r="C97" s="6" t="s">
@@ -2298,11 +2305,11 @@
         <v>1</v>
       </c>
       <c r="E97" s="12"/>
-      <c r="F97" s="77"/>
+      <c r="F97" s="62"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="51"/>
-      <c r="B98" s="53"/>
+      <c r="A98" s="79"/>
+      <c r="B98" s="73"/>
       <c r="C98" s="6" t="s">
         <v>111</v>
       </c>
@@ -2310,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="12"/>
-      <c r="F98" s="77"/>
+      <c r="F98" s="62"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="14"/>
@@ -2318,23 +2325,10 @@
       <c r="C99" s="14"/>
       <c r="D99" s="37"/>
       <c r="E99" s="37"/>
-      <c r="F99" s="69"/>
+      <c r="F99" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B81:B88"/>
-    <mergeCell ref="B89:B96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="A81:A98"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="A45:A54"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="A35:A43"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B45:B48"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="A25:A33"/>
@@ -2343,6 +2337,19 @@
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="A2:A23"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A35:A43"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B81:B88"/>
+    <mergeCell ref="B89:B96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="A81:A98"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="B45:B48"/>
     <mergeCell ref="A56:A73"/>
     <mergeCell ref="B75:B76"/>
     <mergeCell ref="A75:A79"/>
@@ -2409,4 +2416,1242 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24BAAF4C-D1C3-453C-82C4-24EA9D99B0F1}">
+  <dimension ref="A1:I88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="70" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="38">
+        <v>0</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="78"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="78"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="78"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="78"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="78"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="78"/>
+      <c r="B8" s="74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="78"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="35">
+        <v>0</v>
+      </c>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="78"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="78"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="35">
+        <v>0</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="78"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="35">
+        <v>0</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="78"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="35">
+        <v>1</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="78"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="35">
+        <v>1</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="78"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="78"/>
+      <c r="B16" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="45">
+        <v>1</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="78"/>
+      <c r="B17" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="33">
+        <v>1</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="78"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="54"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="22">
+        <v>1</v>
+      </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="84"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="24">
+        <v>0</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="78"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="78"/>
+      <c r="B23" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0</v>
+      </c>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="78"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="29">
+        <v>1</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="78"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="78"/>
+      <c r="B26" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="22">
+        <v>1</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="78"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="24">
+        <v>0</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="79"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="12">
+        <v>1</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="54"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="22">
+        <v>0</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="83"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="24">
+        <v>1</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="78"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="9">
+        <v>1</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="78"/>
+      <c r="B33" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="19">
+        <v>1</v>
+      </c>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="78"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="19">
+        <v>1</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="78"/>
+      <c r="B35" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="22">
+        <v>0</v>
+      </c>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="78"/>
+      <c r="B36" s="72"/>
+      <c r="C36" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="24">
+        <v>1</v>
+      </c>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="78"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="9">
+        <v>1</v>
+      </c>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="79"/>
+      <c r="B38" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="54"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="22">
+        <v>0</v>
+      </c>
+      <c r="E40" s="22"/>
+      <c r="F40" s="55"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="78"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="24">
+        <v>1</v>
+      </c>
+      <c r="E41" s="24"/>
+      <c r="F41" s="56"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="78"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="24">
+        <v>1</v>
+      </c>
+      <c r="E42" s="24"/>
+      <c r="F42" s="56"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="78"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" s="9">
+        <v>1</v>
+      </c>
+      <c r="E43" s="9"/>
+      <c r="F43" s="57"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="78"/>
+      <c r="B44" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="29">
+        <v>0</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="58"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="78"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45" s="35">
+        <v>1</v>
+      </c>
+      <c r="E45" s="35"/>
+      <c r="F45" s="59"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="78"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="35">
+        <v>1</v>
+      </c>
+      <c r="E46" s="35"/>
+      <c r="F46" s="59"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="78"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="11">
+        <v>1</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="60"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="78"/>
+      <c r="B48" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="26">
+        <v>1</v>
+      </c>
+      <c r="E48" s="26"/>
+      <c r="F48" s="61"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="79"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="12">
+        <v>1</v>
+      </c>
+      <c r="E49" s="12"/>
+      <c r="F49" s="62"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="54"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="22">
+        <v>0</v>
+      </c>
+      <c r="E51" s="22"/>
+      <c r="F51" s="55"/>
+    </row>
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="78"/>
+      <c r="B52" s="72"/>
+      <c r="C52" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="24">
+        <v>1</v>
+      </c>
+      <c r="E52" s="24"/>
+      <c r="F52" s="56"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="78"/>
+      <c r="B53" s="72"/>
+      <c r="C53" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="24">
+        <v>0</v>
+      </c>
+      <c r="E53" s="24"/>
+      <c r="F53" s="56"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="78"/>
+      <c r="B54" s="73"/>
+      <c r="C54" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D54" s="9">
+        <v>1</v>
+      </c>
+      <c r="E54" s="9"/>
+      <c r="F54" s="57"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="78"/>
+      <c r="B55" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="33">
+        <v>0</v>
+      </c>
+      <c r="E55" s="33"/>
+      <c r="F55" s="63"/>
+    </row>
+    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="78"/>
+      <c r="B56" s="80"/>
+      <c r="C56" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="35">
+        <v>1</v>
+      </c>
+      <c r="E56" s="35"/>
+      <c r="F56" s="59"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="78"/>
+      <c r="B57" s="80"/>
+      <c r="C57" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" s="35">
+        <v>0</v>
+      </c>
+      <c r="E57" s="35"/>
+      <c r="F57" s="59"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="78"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" s="11">
+        <v>1</v>
+      </c>
+      <c r="E58" s="11"/>
+      <c r="F58" s="60"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="78"/>
+      <c r="B59" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="22">
+        <v>1</v>
+      </c>
+      <c r="E59" s="22"/>
+      <c r="F59" s="55"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="78"/>
+      <c r="B60" s="72"/>
+      <c r="C60" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" s="24">
+        <v>1</v>
+      </c>
+      <c r="E60" s="24"/>
+      <c r="F60" s="56"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="78"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="9">
+        <v>1</v>
+      </c>
+      <c r="E61" s="9"/>
+      <c r="F61" s="57"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="78"/>
+      <c r="B62" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="33">
+        <v>1</v>
+      </c>
+      <c r="E62" s="33"/>
+      <c r="F62" s="63"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="54"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" s="22">
+        <v>1</v>
+      </c>
+      <c r="E64" s="22">
+        <v>0</v>
+      </c>
+      <c r="F64" s="55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="86"/>
+      <c r="B65" s="73"/>
+      <c r="C65" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="9">
+        <v>1</v>
+      </c>
+      <c r="E65" s="9">
+        <v>0</v>
+      </c>
+      <c r="F65" s="57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="86"/>
+      <c r="B66" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" s="13">
+        <v>1</v>
+      </c>
+      <c r="E66" s="13">
+        <v>0</v>
+      </c>
+      <c r="F66" s="65" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="86"/>
+      <c r="B67" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D67" s="45">
+        <v>1</v>
+      </c>
+      <c r="E67" s="45">
+        <v>0</v>
+      </c>
+      <c r="F67" s="66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="87"/>
+      <c r="B68" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="10">
+        <v>1</v>
+      </c>
+      <c r="E68" s="10">
+        <v>0</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="54"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" s="52">
+        <v>0</v>
+      </c>
+      <c r="E70" s="52"/>
+      <c r="F70" s="67"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="78"/>
+      <c r="B71" s="72"/>
+      <c r="C71" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D71" s="8">
+        <v>0</v>
+      </c>
+      <c r="E71" s="8"/>
+      <c r="F71" s="68"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="78"/>
+      <c r="B72" s="72"/>
+      <c r="C72" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D72" s="8">
+        <v>1</v>
+      </c>
+      <c r="E72" s="8"/>
+      <c r="F72" s="68"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="78"/>
+      <c r="B73" s="72"/>
+      <c r="C73" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D73" s="8">
+        <v>1</v>
+      </c>
+      <c r="E73" s="8"/>
+      <c r="F73" s="68"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="78"/>
+      <c r="B74" s="72"/>
+      <c r="C74" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D74" s="8">
+        <v>0</v>
+      </c>
+      <c r="E74" s="8"/>
+      <c r="F74" s="68"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="78"/>
+      <c r="B75" s="72"/>
+      <c r="C75" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D75" s="8">
+        <v>0</v>
+      </c>
+      <c r="E75" s="8"/>
+      <c r="F75" s="68"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="78"/>
+      <c r="B76" s="72"/>
+      <c r="C76" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D76" s="8">
+        <v>1</v>
+      </c>
+      <c r="E76" s="8"/>
+      <c r="F76" s="68"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="78"/>
+      <c r="B77" s="73"/>
+      <c r="C77" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D77" s="9">
+        <v>1</v>
+      </c>
+      <c r="E77" s="9"/>
+      <c r="F77" s="57"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="78"/>
+      <c r="B78" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D78" s="53">
+        <v>0</v>
+      </c>
+      <c r="E78" s="10"/>
+      <c r="F78" s="69"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="78"/>
+      <c r="B79" s="75"/>
+      <c r="C79" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D79" s="19">
+        <v>0</v>
+      </c>
+      <c r="E79" s="10"/>
+      <c r="F79" s="69"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="78"/>
+      <c r="B80" s="75"/>
+      <c r="C80" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D80" s="19">
+        <v>1</v>
+      </c>
+      <c r="E80" s="10"/>
+      <c r="F80" s="69"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="78"/>
+      <c r="B81" s="75"/>
+      <c r="C81" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" s="19">
+        <v>1</v>
+      </c>
+      <c r="E81" s="10"/>
+      <c r="F81" s="69"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="78"/>
+      <c r="B82" s="75"/>
+      <c r="C82" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D82" s="19">
+        <v>0</v>
+      </c>
+      <c r="E82" s="10"/>
+      <c r="F82" s="69"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="78"/>
+      <c r="B83" s="75"/>
+      <c r="C83" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83" s="19">
+        <v>0</v>
+      </c>
+      <c r="E83" s="10"/>
+      <c r="F83" s="69"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="78"/>
+      <c r="B84" s="75"/>
+      <c r="C84" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D84" s="19">
+        <v>1</v>
+      </c>
+      <c r="E84" s="10"/>
+      <c r="F84" s="69"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="78"/>
+      <c r="B85" s="76"/>
+      <c r="C85" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D85" s="11">
+        <v>1</v>
+      </c>
+      <c r="E85" s="11"/>
+      <c r="F85" s="60"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="78"/>
+      <c r="B86" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D86" s="12">
+        <v>1</v>
+      </c>
+      <c r="E86" s="12"/>
+      <c r="F86" s="62"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="79"/>
+      <c r="B87" s="73"/>
+      <c r="C87" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" s="12">
+        <v>1</v>
+      </c>
+      <c r="E87" s="12"/>
+      <c r="F87" s="62"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A70:A87"/>
+    <mergeCell ref="B70:B77"/>
+    <mergeCell ref="B78:B85"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A51:A62"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="A30:A38"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D64:E68 D51:E62 D1:E49 D70:E87 D89:E1048576">
+    <cfRule type="iconSet" priority="6">
+      <iconSet showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="percent" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H4">
+    <cfRule type="iconSet" priority="5">
+      <iconSet showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="percent" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D50:E50">
+    <cfRule type="iconSet" priority="4">
+      <iconSet showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="percent" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:E63">
+    <cfRule type="iconSet" priority="3">
+      <iconSet showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="percent" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69:E69">
+    <cfRule type="iconSet" priority="2">
+      <iconSet showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="percent" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D88:E88">
+    <cfRule type="iconSet" priority="1">
+      <iconSet showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="1"/>
+        <cfvo type="percent" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>